<commit_message>
Latest clinique changes in source code
</commit_message>
<xml_diff>
--- a/src/testData/TestData.xlsx
+++ b/src/testData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView windowHeight="6330" windowWidth="14340" xWindow="0" yWindow="0"/>
+    <workbookView windowHeight="4260" windowWidth="14745" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="5"/>
@@ -12,12 +12,11 @@
     <sheet name="updates" r:id="rId3" sheetId="7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2138" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2185" uniqueCount="474">
   <si>
     <t>Ankit</t>
   </si>
@@ -1324,6 +1323,9 @@
     <t>ankitgoel06@gmail.com</t>
   </si>
   <si>
+    <t>s96508992311111</t>
+  </si>
+  <si>
     <t>WOMEN,MEN,KIDS,BEAUTY,HOMEWARE,BRANDS,GIFTS,DISCOVER,OFFERS,FIRST CITIZEN</t>
   </si>
   <si>
@@ -1336,6 +1338,21 @@
     <t>cxxzg@gmail.com</t>
   </si>
   <si>
+    <t>sdczaz@gmail.com</t>
+  </si>
+  <si>
+    <t>gcfdzax@gmail.com</t>
+  </si>
+  <si>
+    <t>sfhsxazy@gmail.com</t>
+  </si>
+  <si>
+    <t>cdxwzfd@gmail.com</t>
+  </si>
+  <si>
+    <t>s965089923111111</t>
+  </si>
+  <si>
     <t>xgczaf@gmail.com</t>
   </si>
   <si>
@@ -1405,22 +1422,22 @@
     <t>SS_CheckOut_GuestUser_OrderUsingWallets_All</t>
   </si>
   <si>
-    <t>s96508992312</t>
-  </si>
-  <si>
-    <t>s965089923123</t>
-  </si>
-  <si>
-    <t>sddfgfz@gmail.com</t>
-  </si>
-  <si>
-    <t>ggfzax@gmail.com</t>
-  </si>
-  <si>
-    <t>fgbazy@gmail.com</t>
-  </si>
-  <si>
-    <t>dsfghfd@gmail.com</t>
+    <t>SS_CheckOut_GuestUser_EmptyField</t>
+  </si>
+  <si>
+    <t>SS_CartPage_Public_Verify_Edit_Cart_Sameproduct_Functionality</t>
+  </si>
+  <si>
+    <t>Boots</t>
+  </si>
+  <si>
+    <t>SS_ItemDelete_OneItem_CheckOut</t>
+  </si>
+  <si>
+    <t>SS_CheckOut_NewAddress_Clinique</t>
+  </si>
+  <si>
+    <t>BRANDS</t>
   </si>
 </sst>
 </file>
@@ -2044,13 +2061,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CH281"/>
+  <dimension ref="A1:CH282"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
-      <pane activePane="bottomRight" state="frozen" topLeftCell="C146" xSplit="1" ySplit="1"/>
+      <pane activePane="bottomRight" state="frozen" topLeftCell="B107" xSplit="1" ySplit="1"/>
       <selection activeCell="B1" pane="topRight" sqref="B1"/>
       <selection activeCell="A2" pane="bottomLeft" sqref="A2"/>
-      <selection activeCell="A150" pane="bottomRight" sqref="A150"/>
+      <selection activeCell="A116" pane="bottomRight" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4388,7 +4405,7 @@
       <c r="D24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -4479,7 +4496,7 @@
         <v>362</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -6296,7 +6313,7 @@
         <v>264</v>
       </c>
       <c r="AD43" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="AE43" s="1" t="s">
         <v>384</v>
@@ -9748,7 +9765,7 @@
         <v>433</v>
       </c>
       <c r="D78" s="27" t="s">
-        <v>462</v>
+        <v>435</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
@@ -9793,7 +9810,7 @@
       <c r="AS78" s="1"/>
       <c r="AT78" s="1"/>
       <c r="AU78" s="27" t="s">
-        <v>463</v>
+        <v>444</v>
       </c>
       <c r="AV78" s="1"/>
       <c r="AW78" s="1"/>
@@ -13655,28 +13672,28 @@
     </row>
     <row r="116" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>123</v>
+        <v>472</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C116" s="28" t="s">
+      <c r="C116" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="D116" s="27" t="s">
+      <c r="D116" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
       <c r="G116" s="2" t="s">
-        <v>52</v>
+        <v>473</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>322</v>
+        <v>5</v>
       </c>
       <c r="I116" s="1"/>
       <c r="J116" s="2" t="s">
-        <v>424</v>
+        <v>0</v>
       </c>
       <c r="K116" t="s">
         <v>1</v>
@@ -13730,21 +13747,12 @@
       <c r="AX116" s="1"/>
       <c r="AY116" s="1"/>
       <c r="AZ116" s="1"/>
-      <c r="BA116" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BB116" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="BD116" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="BE116" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="BF116" s="2" t="s">
-        <v>128</v>
-      </c>
+      <c r="BA116" s="1"/>
+      <c r="BB116" s="1"/>
+      <c r="BC116" s="1"/>
+      <c r="BD116" s="1"/>
+      <c r="BE116" s="1"/>
+      <c r="BF116" s="1"/>
       <c r="BG116" s="1"/>
       <c r="BH116" s="1"/>
       <c r="BI116" s="1"/>
@@ -13777,7 +13785,7 @@
     </row>
     <row r="117" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>362</v>
@@ -13853,18 +13861,21 @@
       <c r="AY117" s="1"/>
       <c r="AZ117" s="1"/>
       <c r="BA117" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="BB117" s="1"/>
-      <c r="BC117" s="1"/>
-      <c r="BD117" s="1"/>
-      <c r="BE117" s="1"/>
-      <c r="BF117" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="BG117" s="4" t="s">
-        <v>131</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="BB117" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="BD117" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BE117" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="BF117" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BG117" s="1"/>
       <c r="BH117" s="1"/>
       <c r="BI117" s="1"/>
       <c r="BJ117" s="1"/>
@@ -13896,7 +13907,7 @@
     </row>
     <row r="118" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>387</v>
+        <v>129</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>362</v>
@@ -14015,7 +14026,7 @@
     </row>
     <row r="119" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>362</v>
@@ -14077,12 +14088,8 @@
       <c r="AK119" s="1"/>
       <c r="AL119" s="1"/>
       <c r="AM119" s="1"/>
-      <c r="AN119" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="AO119" s="1" t="s">
-        <v>390</v>
-      </c>
+      <c r="AN119" s="1"/>
+      <c r="AO119" s="1"/>
       <c r="AP119" s="1"/>
       <c r="AQ119" s="1"/>
       <c r="AR119" s="1"/>
@@ -14111,14 +14118,10 @@
       <c r="BI119" s="1"/>
       <c r="BJ119" s="1"/>
       <c r="BK119" s="1"/>
-      <c r="BL119" s="1" t="s">
-        <v>393</v>
-      </c>
+      <c r="BL119" s="1"/>
       <c r="BM119" s="1"/>
       <c r="BN119" s="1"/>
-      <c r="BO119" s="1" t="s">
-        <v>394</v>
-      </c>
+      <c r="BO119" s="1"/>
       <c r="BP119" s="1"/>
       <c r="BQ119" s="1"/>
       <c r="BR119" s="1"/>
@@ -14142,7 +14145,7 @@
     </row>
     <row r="120" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>362</v>
@@ -14269,7 +14272,7 @@
     </row>
     <row r="121" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>362</v>
@@ -14396,16 +14399,16 @@
     </row>
     <row r="122" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C122" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>359</v>
+      <c r="C122" s="28" t="s">
+        <v>434</v>
+      </c>
+      <c r="D122" s="27" t="s">
+        <v>2</v>
       </c>
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
@@ -14413,7 +14416,7 @@
         <v>52</v>
       </c>
       <c r="H122" s="3" t="s">
-        <v>410</v>
+        <v>322</v>
       </c>
       <c r="I122" s="1"/>
       <c r="J122" s="2" t="s">
@@ -14523,16 +14526,16 @@
     </row>
     <row r="123" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C123" s="28" t="s">
-        <v>434</v>
-      </c>
-      <c r="D123" s="27" t="s">
-        <v>2</v>
+      <c r="C123" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>359</v>
       </c>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
@@ -14540,7 +14543,7 @@
         <v>52</v>
       </c>
       <c r="H123" s="3" t="s">
-        <v>322</v>
+        <v>410</v>
       </c>
       <c r="I123" s="1"/>
       <c r="J123" s="2" t="s">
@@ -14650,7 +14653,7 @@
     </row>
     <row r="124" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>362</v>
@@ -14777,7 +14780,7 @@
     </row>
     <row r="125" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>362</v>
@@ -14904,7 +14907,7 @@
     </row>
     <row r="126" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>362</v>
@@ -15031,7 +15034,7 @@
     </row>
     <row r="127" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>362</v>
@@ -15158,7 +15161,7 @@
     </row>
     <row r="128" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>362</v>
@@ -15213,10 +15216,9 @@
       <c r="AD128" s="1"/>
       <c r="AE128" s="1"/>
       <c r="AF128" s="1"/>
-      <c r="AG128" s="1">
-        <v>324353454</v>
-      </c>
+      <c r="AG128" s="1"/>
       <c r="AH128" s="1"/>
+      <c r="AI128" s="1"/>
       <c r="AJ128" s="1"/>
       <c r="AK128" s="1"/>
       <c r="AL128" s="1"/>
@@ -15286,7 +15288,7 @@
     </row>
     <row r="129" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>362</v>
@@ -15341,11 +15343,10 @@
       <c r="AD129" s="1"/>
       <c r="AE129" s="1"/>
       <c r="AF129" s="1"/>
-      <c r="AG129" s="1"/>
+      <c r="AG129" s="1">
+        <v>324353454</v>
+      </c>
       <c r="AH129" s="1"/>
-      <c r="AI129" s="1" t="s">
-        <v>421</v>
-      </c>
       <c r="AJ129" s="1"/>
       <c r="AK129" s="1"/>
       <c r="AL129" s="1"/>
@@ -15415,7 +15416,7 @@
     </row>
     <row r="130" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>362</v>
@@ -15472,13 +15473,13 @@
       <c r="AF130" s="1"/>
       <c r="AG130" s="1"/>
       <c r="AH130" s="1"/>
-      <c r="AI130" s="1"/>
+      <c r="AI130" s="1" t="s">
+        <v>421</v>
+      </c>
       <c r="AJ130" s="1"/>
       <c r="AK130" s="1"/>
       <c r="AL130" s="1"/>
-      <c r="AM130" s="26" t="s">
-        <v>420</v>
-      </c>
+      <c r="AM130" s="1"/>
       <c r="AN130" s="1" t="s">
         <v>389</v>
       </c>
@@ -15544,7 +15545,7 @@
     </row>
     <row r="131" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>362</v>
@@ -15603,11 +15604,11 @@
       <c r="AH131" s="1"/>
       <c r="AI131" s="1"/>
       <c r="AJ131" s="1"/>
-      <c r="AK131" s="1" t="s">
-        <v>419</v>
-      </c>
+      <c r="AK131" s="1"/>
       <c r="AL131" s="1"/>
-      <c r="AM131" s="1"/>
+      <c r="AM131" s="26" t="s">
+        <v>420</v>
+      </c>
       <c r="AN131" s="1" t="s">
         <v>389</v>
       </c>
@@ -15673,7 +15674,7 @@
     </row>
     <row r="132" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>362</v>
@@ -15732,7 +15733,9 @@
       <c r="AH132" s="1"/>
       <c r="AI132" s="1"/>
       <c r="AJ132" s="1"/>
-      <c r="AK132" s="1"/>
+      <c r="AK132" s="1" t="s">
+        <v>419</v>
+      </c>
       <c r="AL132" s="1"/>
       <c r="AM132" s="1"/>
       <c r="AN132" s="1" t="s">
@@ -15800,7 +15803,7 @@
     </row>
     <row r="133" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>362</v>
@@ -15927,7 +15930,7 @@
     </row>
     <row r="134" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>362</v>
@@ -16054,7 +16057,7 @@
     </row>
     <row r="135" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>399</v>
+        <v>418</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>362</v>
@@ -16308,7 +16311,7 @@
     </row>
     <row r="137" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>362</v>
@@ -16435,7 +16438,7 @@
     </row>
     <row r="138" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>422</v>
+        <v>400</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>362</v>
@@ -16562,7 +16565,7 @@
     </row>
     <row r="139" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>401</v>
+        <v>422</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>362</v>
@@ -16689,13 +16692,13 @@
     </row>
     <row r="140" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C140" s="26" t="s">
-        <v>403</v>
+      <c r="C140" s="28" t="s">
+        <v>434</v>
       </c>
       <c r="D140" s="27" t="s">
         <v>2</v>
@@ -16816,7 +16819,7 @@
     </row>
     <row r="141" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>362</v>
@@ -16833,7 +16836,7 @@
         <v>52</v>
       </c>
       <c r="H141" s="3" t="s">
-        <v>410</v>
+        <v>322</v>
       </c>
       <c r="I141" s="1"/>
       <c r="J141" s="2" t="s">
@@ -16943,13 +16946,13 @@
     </row>
     <row r="142" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>397</v>
+        <v>408</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C142" s="28" t="s">
-        <v>434</v>
+      <c r="C142" s="26" t="s">
+        <v>403</v>
       </c>
       <c r="D142" s="27" t="s">
         <v>2</v>
@@ -16960,7 +16963,7 @@
         <v>52</v>
       </c>
       <c r="H142" s="3" t="s">
-        <v>322</v>
+        <v>410</v>
       </c>
       <c r="I142" s="1"/>
       <c r="J142" s="2" t="s">
@@ -17070,7 +17073,7 @@
     </row>
     <row r="143" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>362</v>
@@ -17197,7 +17200,7 @@
     </row>
     <row r="144" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>133</v>
+        <v>392</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>362</v>
@@ -17259,8 +17262,12 @@
       <c r="AK144" s="1"/>
       <c r="AL144" s="1"/>
       <c r="AM144" s="1"/>
-      <c r="AN144" s="1"/>
-      <c r="AO144" s="1"/>
+      <c r="AN144" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="AO144" s="1" t="s">
+        <v>390</v>
+      </c>
       <c r="AP144" s="1"/>
       <c r="AQ144" s="1"/>
       <c r="AR144" s="1"/>
@@ -17273,30 +17280,30 @@
       <c r="AY144" s="1"/>
       <c r="AZ144" s="1"/>
       <c r="BA144" s="1" t="s">
-        <v>5</v>
+        <v>130</v>
       </c>
       <c r="BB144" s="1"/>
       <c r="BC144" s="1"/>
       <c r="BD144" s="1"/>
       <c r="BE144" s="1"/>
-      <c r="BF144" s="1"/>
-      <c r="BG144" s="1"/>
-      <c r="BH144" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="BI144" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="BJ144" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="BK144" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="BL144" s="1"/>
+      <c r="BF144" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="BG144" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="BH144" s="1"/>
+      <c r="BI144" s="1"/>
+      <c r="BJ144" s="1"/>
+      <c r="BK144" s="1"/>
+      <c r="BL144" s="1" t="s">
+        <v>393</v>
+      </c>
       <c r="BM144" s="1"/>
       <c r="BN144" s="1"/>
-      <c r="BO144" s="1"/>
+      <c r="BO144" s="1" t="s">
+        <v>394</v>
+      </c>
       <c r="BP144" s="1"/>
       <c r="BQ144" s="1"/>
       <c r="BR144" s="1"/>
@@ -17320,16 +17327,16 @@
     </row>
     <row r="145" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>334</v>
+        <v>133</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C145" s="26" t="s">
-        <v>376</v>
-      </c>
-      <c r="D145" s="26" t="s">
-        <v>359</v>
+      <c r="C145" s="28" t="s">
+        <v>434</v>
+      </c>
+      <c r="D145" s="27" t="s">
+        <v>2</v>
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
@@ -17405,16 +17412,16 @@
       <c r="BF145" s="1"/>
       <c r="BG145" s="1"/>
       <c r="BH145" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="BI145" s="17" t="s">
-        <v>336</v>
-      </c>
-      <c r="BJ145" t="s">
-        <v>338</v>
+        <v>134</v>
+      </c>
+      <c r="BI145" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="BJ145" s="1" t="s">
+        <v>327</v>
       </c>
       <c r="BK145" s="1" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="BL145" s="1"/>
       <c r="BM145" s="1"/>
@@ -17428,39 +17435,31 @@
       <c r="BU145" s="1"/>
       <c r="BV145" s="1"/>
       <c r="BW145" s="1"/>
-      <c r="BX145" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="BY145" s="17" t="s">
-        <v>337</v>
-      </c>
-      <c r="BZ145" t="s">
-        <v>340</v>
-      </c>
-      <c r="CA145" s="1" t="s">
-        <v>341</v>
-      </c>
+      <c r="BX145" s="1"/>
+      <c r="BY145" s="1"/>
+      <c r="BZ145" s="1"/>
+      <c r="CA145" s="1"/>
       <c r="CB145" s="1"/>
       <c r="CC145" s="1"/>
       <c r="CD145" s="1"/>
       <c r="CE145" s="1"/>
       <c r="CF145" s="1"/>
       <c r="CG145" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="146" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>135</v>
+        <v>334</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C146" s="28" t="s">
-        <v>434</v>
-      </c>
-      <c r="D146" s="27" t="s">
-        <v>2</v>
+      <c r="C146" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="D146" s="26" t="s">
+        <v>359</v>
       </c>
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>
@@ -17527,25 +17526,26 @@
       <c r="AY146" s="1"/>
       <c r="AZ146" s="1"/>
       <c r="BA146" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="BB146" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="BD146" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="BE146" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="BF146" s="2" t="s">
-        <v>137</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="BB146" s="1"/>
+      <c r="BC146" s="1"/>
+      <c r="BD146" s="1"/>
+      <c r="BE146" s="1"/>
+      <c r="BF146" s="1"/>
       <c r="BG146" s="1"/>
-      <c r="BH146" s="1"/>
-      <c r="BI146" s="1"/>
-      <c r="BJ146" s="1"/>
-      <c r="BK146" s="1"/>
+      <c r="BH146" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="BI146" s="17" t="s">
+        <v>336</v>
+      </c>
+      <c r="BJ146" t="s">
+        <v>338</v>
+      </c>
+      <c r="BK146" s="1" t="s">
+        <v>339</v>
+      </c>
       <c r="BL146" s="1"/>
       <c r="BM146" s="1"/>
       <c r="BN146" s="1"/>
@@ -17558,10 +17558,18 @@
       <c r="BU146" s="1"/>
       <c r="BV146" s="1"/>
       <c r="BW146" s="1"/>
-      <c r="BX146" s="1"/>
-      <c r="BY146" s="1"/>
-      <c r="BZ146" s="1"/>
-      <c r="CA146" s="1"/>
+      <c r="BX146" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="BY146" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="BZ146" t="s">
+        <v>340</v>
+      </c>
+      <c r="CA146" s="1" t="s">
+        <v>341</v>
+      </c>
       <c r="CB146" s="1"/>
       <c r="CC146" s="1"/>
       <c r="CD146" s="1"/>
@@ -17573,7 +17581,7 @@
     </row>
     <row r="147" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>362</v>
@@ -17649,18 +17657,21 @@
       <c r="AY147" s="1"/>
       <c r="AZ147" s="1"/>
       <c r="BA147" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="BB147" s="1"/>
-      <c r="BC147" s="1"/>
-      <c r="BD147" s="1"/>
-      <c r="BE147" s="1"/>
-      <c r="BF147" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="BG147" s="4" t="s">
-        <v>131</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="BB147" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="BD147" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BE147" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="BF147" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BG147" s="1"/>
       <c r="BH147" s="1"/>
       <c r="BI147" s="1"/>
       <c r="BJ147" s="1"/>
@@ -17687,12 +17698,12 @@
       <c r="CE147" s="1"/>
       <c r="CF147" s="1"/>
       <c r="CG147" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="148" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>362</v>
@@ -17767,25 +17778,23 @@
       <c r="AX148" s="1"/>
       <c r="AY148" s="1"/>
       <c r="AZ148" s="1"/>
-      <c r="BA148" s="1"/>
+      <c r="BA148" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="BB148" s="1"/>
       <c r="BC148" s="1"/>
       <c r="BD148" s="1"/>
       <c r="BE148" s="1"/>
-      <c r="BF148" s="1"/>
-      <c r="BG148" s="1"/>
-      <c r="BH148" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="BI148" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="BJ148" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="BK148" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="BF148" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="BG148" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="BH148" s="1"/>
+      <c r="BI148" s="1"/>
+      <c r="BJ148" s="1"/>
+      <c r="BK148" s="1"/>
       <c r="BL148" s="1"/>
       <c r="BM148" s="1"/>
       <c r="BN148" s="1"/>
@@ -17813,13 +17822,13 @@
     </row>
     <row r="149" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C149" s="1" t="s">
-        <v>326</v>
+      <c r="C149" s="28" t="s">
+        <v>434</v>
       </c>
       <c r="D149" s="27" t="s">
         <v>2</v>
@@ -17888,26 +17897,25 @@
       <c r="AX149" s="1"/>
       <c r="AY149" s="1"/>
       <c r="AZ149" s="1"/>
-      <c r="BA149" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="BB149" s="4" t="s">
+      <c r="BA149" s="1"/>
+      <c r="BB149" s="1"/>
+      <c r="BC149" s="1"/>
+      <c r="BD149" s="1"/>
+      <c r="BE149" s="1"/>
+      <c r="BF149" s="1"/>
+      <c r="BG149" s="1"/>
+      <c r="BH149" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="BI149" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="BD149" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="BE149" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="BF149" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BG149" s="1"/>
-      <c r="BH149" s="1"/>
-      <c r="BI149" s="1"/>
-      <c r="BJ149" s="1"/>
-      <c r="BK149" s="1"/>
+      <c r="BJ149" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="BK149" s="1" t="s">
+        <v>328</v>
+      </c>
       <c r="BL149" s="1"/>
       <c r="BM149" s="1"/>
       <c r="BN149" s="1"/>
@@ -17935,7 +17943,7 @@
     </row>
     <row r="150" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>362</v>
@@ -17943,7 +17951,9 @@
       <c r="C150" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="D150" s="1"/>
+      <c r="D150" s="27" t="s">
+        <v>2</v>
+      </c>
       <c r="E150" s="1"/>
       <c r="F150" s="1"/>
       <c r="G150" s="2" t="s">
@@ -18009,18 +18019,21 @@
       <c r="AY150" s="1"/>
       <c r="AZ150" s="1"/>
       <c r="BA150" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="BB150" s="1"/>
-      <c r="BC150" s="1"/>
-      <c r="BD150" s="1"/>
-      <c r="BE150" s="1"/>
-      <c r="BF150" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="BG150" s="4" t="s">
-        <v>131</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="BB150" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="BD150" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BE150" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="BF150" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BG150" s="1"/>
       <c r="BH150" s="1"/>
       <c r="BI150" s="1"/>
       <c r="BJ150" s="1"/>
@@ -18052,17 +18065,15 @@
     </row>
     <row r="151" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>385</v>
+        <v>142</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C151" s="26" t="s">
-        <v>386</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="C151" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D151" s="1"/>
       <c r="E151" s="1"/>
       <c r="F151" s="1"/>
       <c r="G151" s="2" t="s">
@@ -18147,9 +18158,7 @@
       <c r="BL151" s="1"/>
       <c r="BM151" s="1"/>
       <c r="BN151" s="1"/>
-      <c r="BO151" s="1" t="s">
-        <v>394</v>
-      </c>
+      <c r="BO151" s="1"/>
       <c r="BP151" s="1"/>
       <c r="BQ151" s="1"/>
       <c r="BR151" s="1"/>
@@ -18168,12 +18177,12 @@
       <c r="CE151" s="1"/>
       <c r="CF151" s="1"/>
       <c r="CG151" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="152" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>362</v>
@@ -18265,9 +18274,7 @@
       <c r="BI152" s="1"/>
       <c r="BJ152" s="1"/>
       <c r="BK152" s="1"/>
-      <c r="BL152" s="1" t="s">
-        <v>393</v>
-      </c>
+      <c r="BL152" s="1"/>
       <c r="BM152" s="1"/>
       <c r="BN152" s="1"/>
       <c r="BO152" s="1" t="s">
@@ -18296,7 +18303,7 @@
     </row>
     <row r="153" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>362</v>
@@ -18393,7 +18400,9 @@
       </c>
       <c r="BM153" s="1"/>
       <c r="BN153" s="1"/>
-      <c r="BO153" s="1"/>
+      <c r="BO153" s="1" t="s">
+        <v>394</v>
+      </c>
       <c r="BP153" s="1"/>
       <c r="BQ153" s="1"/>
       <c r="BR153" s="1"/>
@@ -18417,16 +18426,16 @@
     </row>
     <row r="154" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>143</v>
+        <v>397</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C154" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="D154" s="27" t="s">
-        <v>2</v>
+      <c r="C154" s="26" t="s">
+        <v>386</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="E154" s="1"/>
       <c r="F154" s="1"/>
@@ -18492,26 +18501,26 @@
       <c r="AX154" s="1"/>
       <c r="AY154" s="1"/>
       <c r="AZ154" s="1"/>
-      <c r="BA154" s="1"/>
+      <c r="BA154" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="BB154" s="1"/>
       <c r="BC154" s="1"/>
       <c r="BD154" s="1"/>
       <c r="BE154" s="1"/>
-      <c r="BF154" s="1"/>
-      <c r="BG154" s="1"/>
-      <c r="BH154" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="BI154" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="BJ154" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="BK154" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="BL154" s="1"/>
+      <c r="BF154" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="BG154" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="BH154" s="1"/>
+      <c r="BI154" s="1"/>
+      <c r="BJ154" s="1"/>
+      <c r="BK154" s="1"/>
+      <c r="BL154" s="1" t="s">
+        <v>393</v>
+      </c>
       <c r="BM154" s="1"/>
       <c r="BN154" s="1"/>
       <c r="BO154" s="1"/>
@@ -18533,26 +18542,24 @@
       <c r="CE154" s="1"/>
       <c r="CF154" s="1"/>
       <c r="CG154" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="155" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C155" s="26" t="s">
-        <v>464</v>
+      <c r="C155" s="1" t="s">
+        <v>326</v>
       </c>
       <c r="D155" s="27" t="s">
         <v>2</v>
       </c>
       <c r="E155" s="1"/>
-      <c r="F155" s="27" t="s">
-        <v>2</v>
-      </c>
+      <c r="F155" s="1"/>
       <c r="G155" s="2" t="s">
         <v>52</v>
       </c>
@@ -18584,9 +18591,7 @@
       <c r="S155" s="1"/>
       <c r="T155" s="1"/>
       <c r="U155" s="1"/>
-      <c r="V155" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="V155" s="1"/>
       <c r="W155" s="1"/>
       <c r="X155" s="1"/>
       <c r="Y155" s="1"/>
@@ -18597,19 +18602,13 @@
       <c r="AD155" s="1"/>
       <c r="AE155" s="1"/>
       <c r="AF155" s="1"/>
-      <c r="AG155" s="1" t="s">
-        <v>424</v>
-      </c>
+      <c r="AG155" s="1"/>
       <c r="AH155" s="1"/>
-      <c r="AI155" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="AI155" s="1"/>
       <c r="AJ155" s="1"/>
       <c r="AK155" s="1"/>
       <c r="AL155" s="1"/>
-      <c r="AM155" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="AM155" s="1"/>
       <c r="AN155" s="1"/>
       <c r="AO155" s="1"/>
       <c r="AP155" s="1"/>
@@ -18623,26 +18622,25 @@
       <c r="AX155" s="1"/>
       <c r="AY155" s="1"/>
       <c r="AZ155" s="1"/>
-      <c r="BA155" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BB155" s="4" t="s">
+      <c r="BA155" s="1"/>
+      <c r="BB155" s="1"/>
+      <c r="BC155" s="1"/>
+      <c r="BD155" s="1"/>
+      <c r="BE155" s="1"/>
+      <c r="BF155" s="1"/>
+      <c r="BG155" s="1"/>
+      <c r="BH155" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="BI155" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="BD155" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="BE155" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="BF155" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="BG155" s="1"/>
-      <c r="BH155" s="1"/>
-      <c r="BI155" s="1"/>
-      <c r="BJ155" s="1"/>
-      <c r="BK155" s="1"/>
+      <c r="BJ155" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="BK155" s="1" t="s">
+        <v>328</v>
+      </c>
       <c r="BL155" s="1"/>
       <c r="BM155" s="1"/>
       <c r="BN155" s="1"/>
@@ -18670,13 +18668,13 @@
     </row>
     <row r="156" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>362</v>
       </c>
       <c r="C156" s="26" t="s">
-        <v>465</v>
+        <v>440</v>
       </c>
       <c r="D156" s="27" t="s">
         <v>2</v>
@@ -18756,18 +18754,21 @@
       <c r="AY156" s="1"/>
       <c r="AZ156" s="1"/>
       <c r="BA156" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="BB156" s="1"/>
-      <c r="BC156" s="1"/>
-      <c r="BD156" s="1"/>
-      <c r="BE156" s="1"/>
-      <c r="BF156" t="s">
-        <v>147</v>
-      </c>
-      <c r="BG156" s="4" t="s">
-        <v>146</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="BB156" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="BD156" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BE156" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="BF156" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BG156" s="1"/>
       <c r="BH156" s="1"/>
       <c r="BI156" s="1"/>
       <c r="BJ156" s="1"/>
@@ -18799,13 +18800,13 @@
     </row>
     <row r="157" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>362</v>
       </c>
       <c r="C157" s="26" t="s">
-        <v>466</v>
+        <v>441</v>
       </c>
       <c r="D157" s="27" t="s">
         <v>2</v>
@@ -18884,25 +18885,23 @@
       <c r="AX157" s="1"/>
       <c r="AY157" s="1"/>
       <c r="AZ157" s="1"/>
-      <c r="BA157" s="1"/>
+      <c r="BA157" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="BB157" s="1"/>
       <c r="BC157" s="1"/>
       <c r="BD157" s="1"/>
       <c r="BE157" s="1"/>
-      <c r="BF157" s="1"/>
-      <c r="BG157" s="1"/>
-      <c r="BH157" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="BI157" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="BJ157" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="BK157" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="BF157" t="s">
+        <v>147</v>
+      </c>
+      <c r="BG157" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="BH157" s="1"/>
+      <c r="BI157" s="1"/>
+      <c r="BJ157" s="1"/>
+      <c r="BK157" s="1"/>
       <c r="BL157" s="1"/>
       <c r="BM157" s="1"/>
       <c r="BN157" s="1"/>
@@ -18925,18 +18924,18 @@
       <c r="CE157" s="1"/>
       <c r="CF157" s="1"/>
       <c r="CG157" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="158" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>309</v>
+        <v>148</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>362</v>
       </c>
       <c r="C158" s="26" t="s">
-        <v>467</v>
+        <v>442</v>
       </c>
       <c r="D158" s="27" t="s">
         <v>2</v>
@@ -19016,15 +19015,24 @@
       <c r="AY158" s="1"/>
       <c r="AZ158" s="1"/>
       <c r="BA158" s="1"/>
-      <c r="BB158" s="4"/>
-      <c r="BD158" s="2"/>
-      <c r="BE158" s="3"/>
-      <c r="BF158" s="2"/>
+      <c r="BB158" s="1"/>
+      <c r="BC158" s="1"/>
+      <c r="BD158" s="1"/>
+      <c r="BE158" s="1"/>
+      <c r="BF158" s="1"/>
       <c r="BG158" s="1"/>
-      <c r="BH158" s="1"/>
-      <c r="BI158" s="1"/>
-      <c r="BJ158" s="1"/>
-      <c r="BK158" s="1"/>
+      <c r="BH158" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="BI158" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="BJ158" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="BK158" s="1" t="s">
+        <v>328</v>
+      </c>
       <c r="BL158" s="1"/>
       <c r="BM158" s="1"/>
       <c r="BN158" s="1"/>
@@ -19047,36 +19055,60 @@
       <c r="CE158" s="1"/>
       <c r="CF158" s="1"/>
       <c r="CG158" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="159" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A159" s="9" t="s">
-        <v>237</v>
+      <c r="A159" s="2" t="s">
+        <v>309</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C159" s="1"/>
-      <c r="D159" s="1"/>
+      <c r="C159" s="26" t="s">
+        <v>443</v>
+      </c>
+      <c r="D159" s="27" t="s">
+        <v>2</v>
+      </c>
       <c r="E159" s="1"/>
-      <c r="F159" s="1"/>
-      <c r="G159" s="1"/>
-      <c r="H159" s="1"/>
+      <c r="F159" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="G159" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H159" s="3" t="s">
+        <v>322</v>
+      </c>
       <c r="I159" s="1"/>
-      <c r="J159" s="1"/>
-      <c r="K159" s="1"/>
-      <c r="L159" s="1"/>
-      <c r="M159" s="1"/>
-      <c r="N159" s="1"/>
+      <c r="J159" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="K159" t="s">
+        <v>1</v>
+      </c>
+      <c r="L159" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M159" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N159" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="O159" s="1"/>
-      <c r="P159" s="1"/>
+      <c r="P159" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="Q159" s="1"/>
       <c r="R159" s="1"/>
       <c r="S159" s="1"/>
       <c r="T159" s="1"/>
       <c r="U159" s="1"/>
-      <c r="V159" s="1"/>
+      <c r="V159" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="W159" s="1"/>
       <c r="X159" s="1"/>
       <c r="Y159" s="1"/>
@@ -19087,13 +19119,19 @@
       <c r="AD159" s="1"/>
       <c r="AE159" s="1"/>
       <c r="AF159" s="1"/>
-      <c r="AG159" s="1"/>
+      <c r="AG159" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="AH159" s="1"/>
-      <c r="AI159" s="1"/>
+      <c r="AI159" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="AJ159" s="1"/>
       <c r="AK159" s="1"/>
       <c r="AL159" s="1"/>
-      <c r="AM159" s="1"/>
+      <c r="AM159" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="AN159" s="1"/>
       <c r="AO159" s="1"/>
       <c r="AP159" s="1"/>
@@ -19108,14 +19146,13 @@
       <c r="AY159" s="1"/>
       <c r="AZ159" s="1"/>
       <c r="BA159" s="1"/>
-      <c r="BB159" s="1"/>
-      <c r="BC159" s="1"/>
-      <c r="BD159" s="1"/>
-      <c r="BE159" s="1"/>
-      <c r="BF159" s="1"/>
+      <c r="BB159" s="4"/>
+      <c r="BD159" s="2"/>
+      <c r="BE159" s="3"/>
+      <c r="BF159" s="2"/>
       <c r="BG159" s="1"/>
       <c r="BH159" s="1"/>
-      <c r="BI159" s="11"/>
+      <c r="BI159" s="1"/>
       <c r="BJ159" s="1"/>
       <c r="BK159" s="1"/>
       <c r="BL159" s="1"/>
@@ -19139,66 +19176,36 @@
       <c r="CD159" s="1"/>
       <c r="CE159" s="1"/>
       <c r="CF159" s="1"/>
-      <c r="CG159" s="1"/>
+      <c r="CG159" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="160" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A160" s="2" t="s">
-        <v>245</v>
+      <c r="A160" s="9" t="s">
+        <v>237</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C160" s="28" t="s">
-        <v>427</v>
-      </c>
-      <c r="D160" s="11" t="s">
-        <v>359</v>
-      </c>
-      <c r="E160" s="3"/>
-      <c r="F160" s="3"/>
-      <c r="G160" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="H160" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="I160" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="J160" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="K160" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="L160" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="M160" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N160" s="1" t="s">
-        <v>232</v>
-      </c>
+      <c r="C160" s="1"/>
+      <c r="D160" s="1"/>
+      <c r="E160" s="1"/>
+      <c r="F160" s="1"/>
+      <c r="G160" s="1"/>
+      <c r="H160" s="1"/>
+      <c r="I160" s="1"/>
+      <c r="J160" s="1"/>
+      <c r="K160" s="1"/>
+      <c r="L160" s="1"/>
+      <c r="M160" s="1"/>
+      <c r="N160" s="1"/>
       <c r="O160" s="1"/>
-      <c r="P160" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q160" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="R160" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="S160" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="T160" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="U160" s="1" t="s">
-        <v>243</v>
-      </c>
+      <c r="P160" s="1"/>
+      <c r="Q160" s="1"/>
+      <c r="R160" s="1"/>
+      <c r="S160" s="1"/>
+      <c r="T160" s="1"/>
+      <c r="U160" s="1"/>
       <c r="V160" s="1"/>
       <c r="W160" s="1"/>
       <c r="X160" s="1"/>
@@ -19210,9 +19217,7 @@
       <c r="AD160" s="1"/>
       <c r="AE160" s="1"/>
       <c r="AF160" s="1"/>
-      <c r="AG160" s="1" t="s">
-        <v>348</v>
-      </c>
+      <c r="AG160" s="1"/>
       <c r="AH160" s="1"/>
       <c r="AI160" s="1"/>
       <c r="AJ160" s="1"/>
@@ -19232,21 +19237,12 @@
       <c r="AX160" s="1"/>
       <c r="AY160" s="1"/>
       <c r="AZ160" s="1"/>
-      <c r="BA160" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BB160" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="BD160" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="BE160" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="BF160" s="2" t="s">
-        <v>128</v>
-      </c>
+      <c r="BA160" s="1"/>
+      <c r="BB160" s="1"/>
+      <c r="BC160" s="1"/>
+      <c r="BD160" s="1"/>
+      <c r="BE160" s="1"/>
+      <c r="BF160" s="1"/>
       <c r="BG160" s="1"/>
       <c r="BH160" s="1"/>
       <c r="BI160" s="11"/>
@@ -19272,14 +19268,12 @@
       <c r="CC160" s="1"/>
       <c r="CD160" s="1"/>
       <c r="CE160" s="1"/>
-      <c r="CF160" s="18"/>
-      <c r="CG160" t="s">
-        <v>361</v>
-      </c>
+      <c r="CF160" s="1"/>
+      <c r="CG160" s="1"/>
     </row>
     <row r="161" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>362</v>
@@ -19293,22 +19287,22 @@
       <c r="E161" s="3"/>
       <c r="F161" s="3"/>
       <c r="G161" s="3" t="s">
-        <v>5</v>
+        <v>238</v>
       </c>
       <c r="H161" s="1" t="s">
-        <v>5</v>
+        <v>239</v>
       </c>
       <c r="I161" s="1" t="s">
         <v>285</v>
       </c>
       <c r="J161" s="1" t="s">
-        <v>377</v>
+        <v>312</v>
       </c>
       <c r="K161" s="2" t="s">
-        <v>378</v>
+        <v>346</v>
       </c>
       <c r="L161" s="1" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="M161" s="2" t="s">
         <v>27</v>
@@ -19347,7 +19341,7 @@
       <c r="AE161" s="1"/>
       <c r="AF161" s="1"/>
       <c r="AG161" s="1" t="s">
-        <v>379</v>
+        <v>348</v>
       </c>
       <c r="AH161" s="1"/>
       <c r="AI161" s="1"/>
@@ -19410,37 +19404,41 @@
       <c r="CE161" s="1"/>
       <c r="CF161" s="18"/>
       <c r="CG161" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="162" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>362</v>
       </c>
       <c r="C162" s="28" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D162" s="11" t="s">
         <v>359</v>
       </c>
       <c r="E162" s="3"/>
       <c r="F162" s="3"/>
-      <c r="G162" s="3"/>
-      <c r="H162" s="1"/>
+      <c r="G162" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H162" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="I162" s="1" t="s">
         <v>285</v>
       </c>
       <c r="J162" s="1" t="s">
-        <v>312</v>
+        <v>377</v>
       </c>
       <c r="K162" s="2" t="s">
-        <v>346</v>
+        <v>378</v>
       </c>
       <c r="L162" s="1" t="s">
-        <v>313</v>
+        <v>360</v>
       </c>
       <c r="M162" s="2" t="s">
         <v>27</v>
@@ -19479,7 +19477,7 @@
       <c r="AE162" s="1"/>
       <c r="AF162" s="1"/>
       <c r="AG162" s="1" t="s">
-        <v>348</v>
+        <v>379</v>
       </c>
       <c r="AH162" s="1"/>
       <c r="AI162" s="1"/>
@@ -19500,12 +19498,21 @@
       <c r="AX162" s="1"/>
       <c r="AY162" s="1"/>
       <c r="AZ162" s="1"/>
-      <c r="BA162" s="1"/>
-      <c r="BB162" s="1"/>
-      <c r="BC162" s="12"/>
-      <c r="BD162" s="1"/>
-      <c r="BE162" s="1"/>
-      <c r="BF162" s="1"/>
+      <c r="BA162" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="BB162" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="BD162" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BE162" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="BF162" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="BG162" s="1"/>
       <c r="BH162" s="1"/>
       <c r="BI162" s="11"/>
@@ -19538,44 +19545,38 @@
     </row>
     <row r="163" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C163" s="26" t="s">
-        <v>437</v>
-      </c>
-      <c r="D163" s="27" t="s">
-        <v>2</v>
+      <c r="C163" s="28" t="s">
+        <v>428</v>
+      </c>
+      <c r="D163" s="11" t="s">
+        <v>359</v>
       </c>
       <c r="E163" s="3"/>
-      <c r="F163" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G163" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="H163" s="1" t="s">
-        <v>239</v>
-      </c>
+      <c r="F163" s="3"/>
+      <c r="G163" s="3"/>
+      <c r="H163" s="1"/>
       <c r="I163" s="1" t="s">
         <v>285</v>
       </c>
       <c r="J163" s="1" t="s">
-        <v>371</v>
+        <v>312</v>
       </c>
       <c r="K163" s="2" t="s">
-        <v>372</v>
+        <v>346</v>
       </c>
       <c r="L163" s="1" t="s">
-        <v>370</v>
+        <v>313</v>
       </c>
       <c r="M163" s="2" t="s">
-        <v>367</v>
+        <v>27</v>
       </c>
       <c r="N163" s="1" t="s">
-        <v>368</v>
+        <v>232</v>
       </c>
       <c r="O163" s="1"/>
       <c r="P163" s="1" t="s">
@@ -19608,7 +19609,7 @@
       <c r="AE163" s="1"/>
       <c r="AF163" s="1"/>
       <c r="AG163" s="1" t="s">
-        <v>369</v>
+        <v>348</v>
       </c>
       <c r="AH163" s="1"/>
       <c r="AI163" s="1"/>
@@ -19666,20 +19667,22 @@
       </c>
     </row>
     <row r="164" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A164" s="7" t="s">
-        <v>249</v>
+      <c r="A164" s="2" t="s">
+        <v>248</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C164" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="D164" s="11" t="s">
-        <v>359</v>
+      <c r="C164" s="26" t="s">
+        <v>438</v>
+      </c>
+      <c r="D164" s="27" t="s">
+        <v>2</v>
       </c>
       <c r="E164" s="3"/>
-      <c r="F164" s="3"/>
+      <c r="F164" s="27" t="s">
+        <v>2</v>
+      </c>
       <c r="G164" s="3" t="s">
         <v>238</v>
       </c>
@@ -19690,19 +19693,19 @@
         <v>285</v>
       </c>
       <c r="J164" s="1" t="s">
-        <v>312</v>
+        <v>371</v>
       </c>
       <c r="K164" s="2" t="s">
-        <v>346</v>
+        <v>372</v>
       </c>
       <c r="L164" s="1" t="s">
-        <v>313</v>
+        <v>370</v>
       </c>
       <c r="M164" s="2" t="s">
-        <v>27</v>
+        <v>367</v>
       </c>
       <c r="N164" s="1" t="s">
-        <v>232</v>
+        <v>368</v>
       </c>
       <c r="O164" s="1"/>
       <c r="P164" s="1" t="s">
@@ -19735,7 +19738,7 @@
       <c r="AE164" s="1"/>
       <c r="AF164" s="1"/>
       <c r="AG164" s="1" t="s">
-        <v>348</v>
+        <v>369</v>
       </c>
       <c r="AH164" s="1"/>
       <c r="AI164" s="1"/>
@@ -19756,21 +19759,12 @@
       <c r="AX164" s="1"/>
       <c r="AY164" s="1"/>
       <c r="AZ164" s="1"/>
-      <c r="BA164" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="BB164" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="BD164" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="BE164" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="BF164" s="2" t="s">
-        <v>128</v>
-      </c>
+      <c r="BA164" s="1"/>
+      <c r="BB164" s="1"/>
+      <c r="BC164" s="12"/>
+      <c r="BD164" s="1"/>
+      <c r="BE164" s="1"/>
+      <c r="BF164" s="1"/>
       <c r="BG164" s="1"/>
       <c r="BH164" s="1"/>
       <c r="BI164" s="11"/>
@@ -19803,21 +19797,25 @@
     </row>
     <row r="165" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>362</v>
       </c>
       <c r="C165" s="28" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D165" s="11" t="s">
         <v>359</v>
       </c>
       <c r="E165" s="3"/>
       <c r="F165" s="3"/>
-      <c r="G165" s="3"/>
-      <c r="H165" s="1"/>
+      <c r="G165" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="H165" s="1" t="s">
+        <v>239</v>
+      </c>
       <c r="I165" s="1" t="s">
         <v>285</v>
       </c>
@@ -19935,13 +19933,13 @@
     </row>
     <row r="166" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>362</v>
       </c>
       <c r="C166" s="28" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D166" s="11" t="s">
         <v>359</v>
@@ -20067,38 +20065,32 @@
     </row>
     <row r="167" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C167" s="26" t="s">
-        <v>438</v>
-      </c>
-      <c r="D167" s="27" t="s">
-        <v>2</v>
+      <c r="C167" s="28" t="s">
+        <v>431</v>
+      </c>
+      <c r="D167" s="11" t="s">
+        <v>359</v>
       </c>
       <c r="E167" s="3"/>
-      <c r="F167" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G167" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="H167" s="1" t="s">
-        <v>239</v>
-      </c>
+      <c r="F167" s="3"/>
+      <c r="G167" s="3"/>
+      <c r="H167" s="1"/>
       <c r="I167" s="1" t="s">
         <v>285</v>
       </c>
       <c r="J167" s="1" t="s">
-        <v>380</v>
+        <v>312</v>
       </c>
       <c r="K167" s="2" t="s">
-        <v>381</v>
+        <v>346</v>
       </c>
       <c r="L167" s="1" t="s">
-        <v>241</v>
+        <v>313</v>
       </c>
       <c r="M167" s="2" t="s">
         <v>27</v>
@@ -20137,7 +20129,7 @@
       <c r="AE167" s="1"/>
       <c r="AF167" s="1"/>
       <c r="AG167" s="1" t="s">
-        <v>382</v>
+        <v>348</v>
       </c>
       <c r="AH167" s="1"/>
       <c r="AI167" s="1"/>
@@ -20189,14 +20181,14 @@
       <c r="BT167" s="1"/>
       <c r="BU167" s="1"/>
       <c r="BV167" s="1"/>
-      <c r="BW167" s="12"/>
-      <c r="BX167" s="12"/>
-      <c r="BY167" s="12"/>
-      <c r="BZ167" s="12"/>
-      <c r="CA167" s="12"/>
-      <c r="CB167" s="12"/>
-      <c r="CC167" s="12"/>
-      <c r="CD167" s="12"/>
+      <c r="BW167" s="1"/>
+      <c r="BX167" s="1"/>
+      <c r="BY167" s="1"/>
+      <c r="BZ167" s="1"/>
+      <c r="CA167" s="1"/>
+      <c r="CB167" s="1"/>
+      <c r="CC167" s="1"/>
+      <c r="CD167" s="1"/>
       <c r="CE167" s="1"/>
       <c r="CF167" s="18"/>
       <c r="CG167" t="s">
@@ -20205,38 +20197,64 @@
     </row>
     <row r="168" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
-        <v>281</v>
+        <v>252</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C168" s="28" t="s">
-        <v>434</v>
+      <c r="C168" s="26" t="s">
+        <v>439</v>
       </c>
       <c r="D168" s="27" t="s">
         <v>2</v>
       </c>
       <c r="E168" s="3"/>
-      <c r="F168" s="3"/>
+      <c r="F168" s="27" t="s">
+        <v>2</v>
+      </c>
       <c r="G168" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H168" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I168" s="1"/>
-      <c r="J168" s="1"/>
-      <c r="K168" s="2"/>
-      <c r="L168" s="1"/>
-      <c r="M168" s="2"/>
-      <c r="N168" s="1"/>
+        <v>238</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="I168" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J168" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="K168" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="L168" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="M168" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N168" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="O168" s="1"/>
-      <c r="P168" s="1"/>
-      <c r="Q168" s="11"/>
-      <c r="R168" s="10"/>
-      <c r="S168" s="10"/>
-      <c r="T168" s="1"/>
-      <c r="U168" s="1"/>
+      <c r="P168" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q168" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="R168" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="S168" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="T168" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="U168" s="1" t="s">
+        <v>243</v>
+      </c>
       <c r="V168" s="1"/>
       <c r="W168" s="1"/>
       <c r="X168" s="1"/>
@@ -20248,7 +20266,9 @@
       <c r="AD168" s="1"/>
       <c r="AE168" s="1"/>
       <c r="AF168" s="1"/>
-      <c r="AG168" s="1"/>
+      <c r="AG168" s="1" t="s">
+        <v>382</v>
+      </c>
       <c r="AH168" s="1"/>
       <c r="AI168" s="1"/>
       <c r="AJ168" s="1"/>
@@ -20268,18 +20288,24 @@
       <c r="AX168" s="1"/>
       <c r="AY168" s="1"/>
       <c r="AZ168" s="1"/>
-      <c r="BA168" s="1"/>
-      <c r="BB168" s="4"/>
-      <c r="BD168" s="2"/>
-      <c r="BE168" s="3"/>
-      <c r="BF168" s="2"/>
+      <c r="BA168" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="BB168" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="BD168" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BE168" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="BF168" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="BG168" s="1"/>
-      <c r="BH168" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="BI168" s="11" t="s">
-        <v>349</v>
-      </c>
+      <c r="BH168" s="1"/>
+      <c r="BI168" s="11"/>
       <c r="BJ168" s="1"/>
       <c r="BK168" s="1"/>
       <c r="BL168" s="1"/>
@@ -20304,18 +20330,18 @@
       <c r="CE168" s="1"/>
       <c r="CF168" s="18"/>
       <c r="CG168" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="169" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C169" s="1" t="s">
-        <v>326</v>
+      <c r="C169" s="28" t="s">
+        <v>434</v>
       </c>
       <c r="D169" s="27" t="s">
         <v>2</v>
@@ -20329,28 +20355,16 @@
         <v>58</v>
       </c>
       <c r="I169" s="1"/>
-      <c r="J169" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="K169" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L169" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M169" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N169" s="1" t="s">
-        <v>232</v>
-      </c>
+      <c r="J169" s="1"/>
+      <c r="K169" s="2"/>
+      <c r="L169" s="1"/>
+      <c r="M169" s="2"/>
+      <c r="N169" s="1"/>
       <c r="O169" s="1"/>
-      <c r="P169" s="1" t="s">
-        <v>122</v>
-      </c>
+      <c r="P169" s="1"/>
       <c r="Q169" s="11"/>
-      <c r="R169" s="1"/>
-      <c r="S169" s="1"/>
+      <c r="R169" s="10"/>
+      <c r="S169" s="10"/>
       <c r="T169" s="1"/>
       <c r="U169" s="1"/>
       <c r="V169" s="1"/>
@@ -20384,9 +20398,7 @@
       <c r="AX169" s="1"/>
       <c r="AY169" s="1"/>
       <c r="AZ169" s="1"/>
-      <c r="BA169" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="BA169" s="1"/>
       <c r="BB169" s="4"/>
       <c r="BD169" s="2"/>
       <c r="BE169" s="3"/>
@@ -20396,14 +20408,10 @@
         <v>282</v>
       </c>
       <c r="BI169" s="11" t="s">
-        <v>283</v>
-      </c>
-      <c r="BJ169" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="BK169" s="1" t="s">
-        <v>350</v>
-      </c>
+        <v>349</v>
+      </c>
+      <c r="BJ169" s="1"/>
+      <c r="BK169" s="1"/>
       <c r="BL169" s="1"/>
       <c r="BM169" s="1"/>
       <c r="BN169" s="1"/>
@@ -20429,9 +20437,9 @@
         <v>361</v>
       </c>
     </row>
-    <row ht="30" r="170" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>362</v>
@@ -20444,39 +20452,37 @@
       </c>
       <c r="E170" s="3"/>
       <c r="F170" s="3"/>
-      <c r="G170" s="3"/>
-      <c r="H170" s="3"/>
-      <c r="I170" s="1" t="s">
-        <v>285</v>
-      </c>
+      <c r="G170" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H170" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I170" s="1"/>
       <c r="J170" s="2" t="s">
-        <v>289</v>
+        <v>424</v>
       </c>
       <c r="K170" s="2" t="s">
-        <v>290</v>
+        <v>1</v>
       </c>
       <c r="L170" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="M170" s="2"/>
-      <c r="N170" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="M170" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N170" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="O170" s="1"/>
-      <c r="P170" s="1"/>
-      <c r="Q170" s="11" t="s">
-        <v>287</v>
-      </c>
-      <c r="R170" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="S170" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="T170" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="U170" s="1" t="s">
-        <v>293</v>
-      </c>
+      <c r="P170" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q170" s="11"/>
+      <c r="R170" s="1"/>
+      <c r="S170" s="1"/>
+      <c r="T170" s="1"/>
+      <c r="U170" s="1"/>
       <c r="V170" s="1"/>
       <c r="W170" s="1"/>
       <c r="X170" s="1"/>
@@ -20488,9 +20494,7 @@
       <c r="AD170" s="1"/>
       <c r="AE170" s="1"/>
       <c r="AF170" s="1"/>
-      <c r="AG170" s="1" t="s">
-        <v>286</v>
-      </c>
+      <c r="AG170" s="1"/>
       <c r="AH170" s="1"/>
       <c r="AI170" s="1"/>
       <c r="AJ170" s="1"/>
@@ -20510,20 +20514,28 @@
       <c r="AX170" s="1"/>
       <c r="AY170" s="1"/>
       <c r="AZ170" s="1"/>
-      <c r="BA170" s="1"/>
+      <c r="BA170" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="BB170" s="4"/>
       <c r="BD170" s="2"/>
       <c r="BE170" s="3"/>
       <c r="BF170" s="2"/>
       <c r="BG170" s="1"/>
-      <c r="BH170" s="1"/>
-      <c r="BI170" s="11"/>
-      <c r="BJ170" s="1"/>
-      <c r="BK170" s="1"/>
+      <c r="BH170" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="BI170" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="BJ170" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="BK170" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="BL170" s="1"/>
-      <c r="BM170" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="BM170" s="1"/>
       <c r="BN170" s="1"/>
       <c r="BO170" s="1"/>
       <c r="BP170" s="1"/>
@@ -20548,51 +20560,53 @@
       </c>
     </row>
     <row ht="30" r="171" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A171" s="2" t="s">
-        <v>440</v>
+      <c r="A171" s="7" t="s">
+        <v>284</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>362</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="D171" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D171" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E171" s="1"/>
-      <c r="F171" s="1"/>
-      <c r="G171" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H171" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="I171" s="1"/>
+      <c r="E171" s="3"/>
+      <c r="F171" s="3"/>
+      <c r="G171" s="3"/>
+      <c r="H171" s="3"/>
+      <c r="I171" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="J171" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K171" t="s">
-        <v>1</v>
+        <v>289</v>
+      </c>
+      <c r="K171" s="2" t="s">
+        <v>290</v>
       </c>
       <c r="L171" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M171" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N171" s="1" t="s">
-        <v>232</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="M171" s="2"/>
+      <c r="N171" s="1"/>
       <c r="O171" s="1"/>
-      <c r="P171" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q171" s="1"/>
-      <c r="R171" s="1"/>
-      <c r="S171" s="1"/>
-      <c r="T171" s="1"/>
-      <c r="U171" s="1"/>
+      <c r="P171" s="1"/>
+      <c r="Q171" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="R171" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="S171" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="T171" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="U171" s="1" t="s">
+        <v>293</v>
+      </c>
       <c r="V171" s="1"/>
       <c r="W171" s="1"/>
       <c r="X171" s="1"/>
@@ -20604,7 +20618,9 @@
       <c r="AD171" s="1"/>
       <c r="AE171" s="1"/>
       <c r="AF171" s="1"/>
-      <c r="AG171" s="1"/>
+      <c r="AG171" s="1" t="s">
+        <v>286</v>
+      </c>
       <c r="AH171" s="1"/>
       <c r="AI171" s="1"/>
       <c r="AJ171" s="1"/>
@@ -20624,25 +20640,20 @@
       <c r="AX171" s="1"/>
       <c r="AY171" s="1"/>
       <c r="AZ171" s="1"/>
-      <c r="BA171" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="BB171" s="1"/>
-      <c r="BC171" s="1"/>
-      <c r="BD171" s="1"/>
-      <c r="BE171" s="1"/>
-      <c r="BF171" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="BG171" s="4" t="s">
-        <v>443</v>
-      </c>
+      <c r="BA171" s="1"/>
+      <c r="BB171" s="4"/>
+      <c r="BD171" s="2"/>
+      <c r="BE171" s="3"/>
+      <c r="BF171" s="2"/>
+      <c r="BG171" s="1"/>
       <c r="BH171" s="1"/>
-      <c r="BI171" s="1"/>
+      <c r="BI171" s="11"/>
       <c r="BJ171" s="1"/>
       <c r="BK171" s="1"/>
       <c r="BL171" s="1"/>
-      <c r="BM171" s="1"/>
+      <c r="BM171" s="1" t="s">
+        <v>291</v>
+      </c>
       <c r="BN171" s="1"/>
       <c r="BO171" s="1"/>
       <c r="BP171" s="1"/>
@@ -20652,23 +20663,23 @@
       <c r="BT171" s="1"/>
       <c r="BU171" s="1"/>
       <c r="BV171" s="1"/>
-      <c r="BW171" s="1"/>
-      <c r="BX171" s="1"/>
-      <c r="BY171" s="1"/>
-      <c r="BZ171" s="1"/>
-      <c r="CA171" s="1"/>
-      <c r="CB171" s="1"/>
-      <c r="CC171" s="1"/>
-      <c r="CD171" s="1"/>
+      <c r="BW171" s="12"/>
+      <c r="BX171" s="12"/>
+      <c r="BY171" s="12"/>
+      <c r="BZ171" s="12"/>
+      <c r="CA171" s="12"/>
+      <c r="CB171" s="12"/>
+      <c r="CC171" s="12"/>
+      <c r="CD171" s="12"/>
       <c r="CE171" s="1"/>
-      <c r="CF171" s="1"/>
+      <c r="CF171" s="18"/>
       <c r="CG171" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row ht="30" r="172" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>362</v>
@@ -20744,17 +20755,17 @@
       <c r="AY172" s="1"/>
       <c r="AZ172" s="1"/>
       <c r="BA172" s="1" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="BB172" s="1"/>
       <c r="BC172" s="1"/>
       <c r="BD172" s="1"/>
       <c r="BE172" s="1"/>
       <c r="BF172" s="1" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="BG172" s="4" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="BH172" s="1"/>
       <c r="BI172" s="1"/>
@@ -20787,7 +20798,7 @@
     </row>
     <row ht="30" r="173" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>362</v>
@@ -20863,17 +20874,17 @@
       <c r="AY173" s="1"/>
       <c r="AZ173" s="1"/>
       <c r="BA173" s="1" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="BB173" s="1"/>
       <c r="BC173" s="1"/>
       <c r="BD173" s="1"/>
       <c r="BE173" s="1"/>
       <c r="BF173" s="1" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="BG173" s="4" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="BH173" s="1"/>
       <c r="BI173" s="1"/>
@@ -20904,9 +20915,9 @@
         <v>363</v>
       </c>
     </row>
-    <row r="174" spans="1:85" x14ac:dyDescent="0.25">
+    <row ht="30" r="174" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>362</v>
@@ -20982,17 +20993,17 @@
       <c r="AY174" s="1"/>
       <c r="AZ174" s="1"/>
       <c r="BA174" s="1" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="BB174" s="1"/>
       <c r="BC174" s="1"/>
       <c r="BD174" s="1"/>
       <c r="BE174" s="1"/>
       <c r="BF174" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="BG174" s="4" t="s">
         <v>449</v>
-      </c>
-      <c r="BG174" s="4" t="s">
-        <v>443</v>
       </c>
       <c r="BH174" s="1"/>
       <c r="BI174" s="1"/>
@@ -21025,7 +21036,7 @@
     </row>
     <row r="175" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>362</v>
@@ -21101,17 +21112,17 @@
       <c r="AY175" s="1"/>
       <c r="AZ175" s="1"/>
       <c r="BA175" s="1" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="BB175" s="1"/>
       <c r="BC175" s="1"/>
       <c r="BD175" s="1"/>
       <c r="BE175" s="1"/>
       <c r="BF175" s="1" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="BG175" s="4" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="BH175" s="1"/>
       <c r="BI175" s="1"/>
@@ -21144,7 +21155,7 @@
     </row>
     <row r="176" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>362</v>
@@ -21220,17 +21231,17 @@
       <c r="AY176" s="1"/>
       <c r="AZ176" s="1"/>
       <c r="BA176" s="1" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="BB176" s="1"/>
       <c r="BC176" s="1"/>
       <c r="BD176" s="1"/>
       <c r="BE176" s="1"/>
       <c r="BF176" s="1" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="BG176" s="4" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="BH176" s="1"/>
       <c r="BI176" s="1"/>
@@ -21261,17 +21272,19 @@
         <v>363</v>
       </c>
     </row>
-    <row ht="30" r="177" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>362</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="D177" s="1"/>
+        <v>434</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="E177" s="1"/>
       <c r="F177" s="1"/>
       <c r="G177" s="2" t="s">
@@ -21337,17 +21350,17 @@
       <c r="AY177" s="1"/>
       <c r="AZ177" s="1"/>
       <c r="BA177" s="1" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="BB177" s="1"/>
       <c r="BC177" s="1"/>
       <c r="BD177" s="1"/>
       <c r="BE177" s="1"/>
       <c r="BF177" s="1" t="s">
-        <v>442</v>
+        <v>459</v>
       </c>
       <c r="BG177" s="4" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="BH177" s="1"/>
       <c r="BI177" s="1"/>
@@ -21380,7 +21393,7 @@
     </row>
     <row ht="30" r="178" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>362</v>
@@ -21454,17 +21467,17 @@
       <c r="AY178" s="1"/>
       <c r="AZ178" s="1"/>
       <c r="BA178" s="1" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="BB178" s="1"/>
       <c r="BC178" s="1"/>
       <c r="BD178" s="1"/>
       <c r="BE178" s="1"/>
       <c r="BF178" s="1" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="BG178" s="4" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="BH178" s="1"/>
       <c r="BI178" s="1"/>
@@ -21497,7 +21510,7 @@
     </row>
     <row ht="30" r="179" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>362</v>
@@ -21571,17 +21584,17 @@
       <c r="AY179" s="1"/>
       <c r="AZ179" s="1"/>
       <c r="BA179" s="1" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="BB179" s="1"/>
       <c r="BC179" s="1"/>
       <c r="BD179" s="1"/>
       <c r="BE179" s="1"/>
       <c r="BF179" s="1" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="BG179" s="4" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="BH179" s="1"/>
       <c r="BI179" s="1"/>
@@ -21612,9 +21625,9 @@
         <v>363</v>
       </c>
     </row>
-    <row r="180" spans="1:85" x14ac:dyDescent="0.25">
+    <row ht="30" r="180" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>362</v>
@@ -21688,17 +21701,17 @@
       <c r="AY180" s="1"/>
       <c r="AZ180" s="1"/>
       <c r="BA180" s="1" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="BB180" s="1"/>
       <c r="BC180" s="1"/>
       <c r="BD180" s="1"/>
       <c r="BE180" s="1"/>
       <c r="BF180" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="BG180" s="4" t="s">
         <v>449</v>
-      </c>
-      <c r="BG180" s="4" t="s">
-        <v>443</v>
       </c>
       <c r="BH180" s="1"/>
       <c r="BI180" s="1"/>
@@ -21731,7 +21744,7 @@
     </row>
     <row r="181" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>362</v>
@@ -21805,17 +21818,17 @@
       <c r="AY181" s="1"/>
       <c r="AZ181" s="1"/>
       <c r="BA181" s="1" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="BB181" s="1"/>
       <c r="BC181" s="1"/>
       <c r="BD181" s="1"/>
       <c r="BE181" s="1"/>
       <c r="BF181" s="1" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="BG181" s="4" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="BH181" s="1"/>
       <c r="BI181" s="1"/>
@@ -21848,7 +21861,7 @@
     </row>
     <row r="182" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>362</v>
@@ -21922,17 +21935,17 @@
       <c r="AY182" s="1"/>
       <c r="AZ182" s="1"/>
       <c r="BA182" s="1" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="BB182" s="1"/>
       <c r="BC182" s="1"/>
       <c r="BD182" s="1"/>
       <c r="BE182" s="1"/>
       <c r="BF182" s="1" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="BG182" s="4" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="BH182" s="1"/>
       <c r="BI182" s="1"/>
@@ -21960,22 +21973,20 @@
       <c r="CE182" s="1"/>
       <c r="CF182" s="1"/>
       <c r="CG182" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="183" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>362</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="D183" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="D183" s="1"/>
       <c r="E183" s="1"/>
       <c r="F183" s="1"/>
       <c r="G183" s="2" t="s">
@@ -22041,14 +22052,18 @@
       <c r="AY183" s="1"/>
       <c r="AZ183" s="1"/>
       <c r="BA183" s="1" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="BB183" s="1"/>
       <c r="BC183" s="1"/>
       <c r="BD183" s="1"/>
       <c r="BE183" s="1"/>
-      <c r="BF183" s="1"/>
-      <c r="BG183" s="4"/>
+      <c r="BF183" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="BG183" s="4" t="s">
+        <v>449</v>
+      </c>
       <c r="BH183" s="1"/>
       <c r="BI183" s="1"/>
       <c r="BJ183" s="1"/>
@@ -22075,20 +22090,22 @@
       <c r="CE183" s="1"/>
       <c r="CF183" s="1"/>
       <c r="CG183" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="184" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>362</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="D184" s="1"/>
+        <v>434</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="E184" s="1"/>
       <c r="F184" s="1"/>
       <c r="G184" s="2" t="s">
@@ -22154,15 +22171,13 @@
       <c r="AY184" s="1"/>
       <c r="AZ184" s="1"/>
       <c r="BA184" s="1" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="BB184" s="1"/>
       <c r="BC184" s="1"/>
       <c r="BD184" s="1"/>
       <c r="BE184" s="1"/>
-      <c r="BF184" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="BF184" s="1"/>
       <c r="BG184" s="4"/>
       <c r="BH184" s="1"/>
       <c r="BI184" s="1"/>
@@ -22194,22 +22209,44 @@
       </c>
     </row>
     <row r="185" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A185" s="7"/>
-      <c r="B185" s="1"/>
-      <c r="C185" s="1"/>
+      <c r="A185" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="D185" s="1"/>
       <c r="E185" s="1"/>
       <c r="F185" s="1"/>
-      <c r="G185" s="1"/>
-      <c r="H185" s="1"/>
+      <c r="G185" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H185" s="3" t="s">
+        <v>322</v>
+      </c>
       <c r="I185" s="1"/>
-      <c r="J185" s="1"/>
-      <c r="K185" s="1"/>
-      <c r="L185" s="1"/>
-      <c r="M185" s="1"/>
-      <c r="N185" s="1"/>
+      <c r="J185" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K185" t="s">
+        <v>1</v>
+      </c>
+      <c r="L185" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M185" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N185" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="O185" s="1"/>
-      <c r="P185" s="1"/>
+      <c r="P185" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="Q185" s="1"/>
       <c r="R185" s="1"/>
       <c r="S185" s="1"/>
@@ -22246,15 +22283,19 @@
       <c r="AX185" s="1"/>
       <c r="AY185" s="1"/>
       <c r="AZ185" s="1"/>
-      <c r="BA185" s="1"/>
+      <c r="BA185" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="BB185" s="1"/>
       <c r="BC185" s="1"/>
       <c r="BD185" s="1"/>
       <c r="BE185" s="1"/>
-      <c r="BF185" s="1"/>
-      <c r="BG185" s="1"/>
+      <c r="BF185" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="BG185" s="4"/>
       <c r="BH185" s="1"/>
-      <c r="BI185" s="11"/>
+      <c r="BI185" s="1"/>
       <c r="BJ185" s="1"/>
       <c r="BK185" s="1"/>
       <c r="BL185" s="1"/>
@@ -22278,25 +22319,49 @@
       <c r="CD185" s="1"/>
       <c r="CE185" s="1"/>
       <c r="CF185" s="1"/>
-      <c r="CG185" s="1"/>
+      <c r="CG185" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="186" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A186" s="7"/>
-      <c r="B186" s="1"/>
-      <c r="C186" s="1"/>
+      <c r="A186" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="D186" s="1"/>
       <c r="E186" s="1"/>
       <c r="F186" s="1"/>
-      <c r="G186" s="1"/>
-      <c r="H186" s="1"/>
+      <c r="G186" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H186" s="3" t="s">
+        <v>322</v>
+      </c>
       <c r="I186" s="1"/>
-      <c r="J186" s="1"/>
-      <c r="K186" s="1"/>
-      <c r="L186" s="1"/>
-      <c r="M186" s="1"/>
-      <c r="N186" s="1"/>
+      <c r="J186" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K186" t="s">
+        <v>1</v>
+      </c>
+      <c r="L186" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M186" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N186" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="O186" s="1"/>
-      <c r="P186" s="1"/>
+      <c r="P186" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="Q186" s="1"/>
       <c r="R186" s="1"/>
       <c r="S186" s="1"/>
@@ -22333,15 +22398,21 @@
       <c r="AX186" s="1"/>
       <c r="AY186" s="1"/>
       <c r="AZ186" s="1"/>
-      <c r="BA186" s="1"/>
+      <c r="BA186" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="BB186" s="1"/>
       <c r="BC186" s="1"/>
       <c r="BD186" s="1"/>
       <c r="BE186" s="1"/>
-      <c r="BF186" s="1"/>
-      <c r="BG186" s="1"/>
+      <c r="BF186" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="BG186" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="BH186" s="1"/>
-      <c r="BI186" s="11"/>
+      <c r="BI186" s="1"/>
       <c r="BJ186" s="1"/>
       <c r="BK186" s="1"/>
       <c r="BL186" s="1"/>
@@ -22365,17 +22436,27 @@
       <c r="CD186" s="1"/>
       <c r="CE186" s="1"/>
       <c r="CF186" s="1"/>
-      <c r="CG186" s="1"/>
+      <c r="CG186" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="187" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A187" s="7"/>
-      <c r="B187" s="1"/>
-      <c r="C187" s="1"/>
+      <c r="A187" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C187" s="11"/>
       <c r="D187" s="1"/>
       <c r="E187" s="1"/>
       <c r="F187" s="1"/>
-      <c r="G187" s="1"/>
-      <c r="H187" s="1"/>
+      <c r="G187" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H187" s="1" t="s">
+        <v>470</v>
+      </c>
       <c r="I187" s="1"/>
       <c r="J187" s="1"/>
       <c r="K187" s="1"/>
@@ -22451,26 +22532,50 @@
       <c r="CC187" s="1"/>
       <c r="CD187" s="1"/>
       <c r="CE187" s="1"/>
-      <c r="CF187" s="1"/>
-      <c r="CG187" s="1"/>
+      <c r="CF187" s="18"/>
+      <c r="CG187" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="188" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A188" s="7"/>
-      <c r="B188" s="1"/>
-      <c r="C188" s="11"/>
+      <c r="A188" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="D188" s="1"/>
       <c r="E188" s="1"/>
       <c r="F188" s="1"/>
-      <c r="G188" s="1"/>
-      <c r="H188" s="1"/>
+      <c r="G188" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H188" s="3" t="s">
+        <v>470</v>
+      </c>
       <c r="I188" s="1"/>
-      <c r="J188" s="1"/>
-      <c r="K188" s="1"/>
-      <c r="L188" s="1"/>
-      <c r="M188" s="1"/>
-      <c r="N188" s="1"/>
+      <c r="J188" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K188" t="s">
+        <v>1</v>
+      </c>
+      <c r="L188" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M188" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N188" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="O188" s="1"/>
-      <c r="P188" s="1"/>
+      <c r="P188" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="Q188" s="1"/>
       <c r="R188" s="1"/>
       <c r="S188" s="1"/>
@@ -22513,9 +22618,9 @@
       <c r="BD188" s="1"/>
       <c r="BE188" s="1"/>
       <c r="BF188" s="1"/>
-      <c r="BG188" s="1"/>
+      <c r="BG188" s="4"/>
       <c r="BH188" s="1"/>
-      <c r="BI188" s="11"/>
+      <c r="BI188" s="1"/>
       <c r="BJ188" s="1"/>
       <c r="BK188" s="1"/>
       <c r="BL188" s="1"/>
@@ -22539,7 +22644,9 @@
       <c r="CD188" s="1"/>
       <c r="CE188" s="1"/>
       <c r="CF188" s="1"/>
-      <c r="CG188" s="1"/>
+      <c r="CG188" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="189" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A189" s="7"/>
@@ -24282,91 +24389,91 @@
       <c r="CG208" s="1"/>
     </row>
     <row r="209" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A209" s="8"/>
-      <c r="B209" s="2"/>
-      <c r="C209" s="3"/>
-      <c r="D209" s="2"/>
-      <c r="E209" s="2"/>
-      <c r="F209" s="2"/>
-      <c r="G209" s="2"/>
-      <c r="H209" s="2"/>
-      <c r="I209" s="2"/>
-      <c r="J209" s="2"/>
-      <c r="K209" s="2"/>
-      <c r="L209" s="2"/>
-      <c r="M209" s="2"/>
-      <c r="N209" s="2"/>
-      <c r="O209" s="2"/>
-      <c r="P209" s="2"/>
-      <c r="Q209" s="2"/>
-      <c r="R209" s="2"/>
-      <c r="S209" s="2"/>
-      <c r="T209" s="2"/>
-      <c r="U209" s="2"/>
-      <c r="V209" s="2"/>
-      <c r="W209" s="2"/>
-      <c r="X209" s="2"/>
-      <c r="Y209" s="2"/>
-      <c r="Z209" s="2"/>
-      <c r="AA209" s="2"/>
-      <c r="AB209" s="2"/>
-      <c r="AC209" s="2"/>
-      <c r="AD209" s="2"/>
-      <c r="AE209" s="2"/>
-      <c r="AF209" s="2"/>
-      <c r="AG209" s="2"/>
-      <c r="AH209" s="2"/>
-      <c r="AI209" s="2"/>
-      <c r="AJ209" s="2"/>
-      <c r="AK209" s="2"/>
-      <c r="AL209" s="2"/>
-      <c r="AM209" s="2"/>
-      <c r="AN209" s="2"/>
-      <c r="AO209" s="2"/>
-      <c r="AP209" s="2"/>
-      <c r="AQ209" s="2"/>
-      <c r="AR209" s="2"/>
-      <c r="AS209" s="2"/>
-      <c r="AT209" s="2"/>
-      <c r="AU209" s="2"/>
-      <c r="AV209" s="2"/>
-      <c r="AW209" s="2"/>
-      <c r="AX209" s="2"/>
-      <c r="AY209" s="2"/>
-      <c r="AZ209" s="2"/>
-      <c r="BA209" s="2"/>
-      <c r="BB209" s="2"/>
-      <c r="BC209" s="2"/>
-      <c r="BD209" s="2"/>
-      <c r="BE209" s="2"/>
-      <c r="BF209" s="2"/>
-      <c r="BG209" s="2"/>
-      <c r="BH209" s="2"/>
-      <c r="BI209" s="3"/>
-      <c r="BJ209" s="2"/>
-      <c r="BK209" s="2"/>
-      <c r="BL209" s="2"/>
-      <c r="BM209" s="2"/>
-      <c r="BN209" s="2"/>
-      <c r="BO209" s="2"/>
-      <c r="BP209" s="2"/>
-      <c r="BQ209" s="2"/>
-      <c r="BR209" s="2"/>
-      <c r="BS209" s="2"/>
-      <c r="BT209" s="2"/>
-      <c r="BU209" s="2"/>
-      <c r="BV209" s="2"/>
-      <c r="BW209" s="2"/>
-      <c r="BX209" s="2"/>
-      <c r="BY209" s="2"/>
-      <c r="BZ209" s="2"/>
-      <c r="CA209" s="2"/>
-      <c r="CB209" s="2"/>
-      <c r="CC209" s="2"/>
-      <c r="CD209" s="2"/>
-      <c r="CE209" s="2"/>
-      <c r="CF209" s="2"/>
-      <c r="CG209" s="2"/>
+      <c r="A209" s="7"/>
+      <c r="B209" s="1"/>
+      <c r="C209" s="11"/>
+      <c r="D209" s="1"/>
+      <c r="E209" s="1"/>
+      <c r="F209" s="1"/>
+      <c r="G209" s="1"/>
+      <c r="H209" s="1"/>
+      <c r="I209" s="1"/>
+      <c r="J209" s="1"/>
+      <c r="K209" s="1"/>
+      <c r="L209" s="1"/>
+      <c r="M209" s="1"/>
+      <c r="N209" s="1"/>
+      <c r="O209" s="1"/>
+      <c r="P209" s="1"/>
+      <c r="Q209" s="1"/>
+      <c r="R209" s="1"/>
+      <c r="S209" s="1"/>
+      <c r="T209" s="1"/>
+      <c r="U209" s="1"/>
+      <c r="V209" s="1"/>
+      <c r="W209" s="1"/>
+      <c r="X209" s="1"/>
+      <c r="Y209" s="1"/>
+      <c r="Z209" s="1"/>
+      <c r="AA209" s="1"/>
+      <c r="AB209" s="1"/>
+      <c r="AC209" s="1"/>
+      <c r="AD209" s="1"/>
+      <c r="AE209" s="1"/>
+      <c r="AF209" s="1"/>
+      <c r="AG209" s="1"/>
+      <c r="AH209" s="1"/>
+      <c r="AI209" s="1"/>
+      <c r="AJ209" s="1"/>
+      <c r="AK209" s="1"/>
+      <c r="AL209" s="1"/>
+      <c r="AM209" s="1"/>
+      <c r="AN209" s="1"/>
+      <c r="AO209" s="1"/>
+      <c r="AP209" s="1"/>
+      <c r="AQ209" s="1"/>
+      <c r="AR209" s="1"/>
+      <c r="AS209" s="1"/>
+      <c r="AT209" s="1"/>
+      <c r="AU209" s="1"/>
+      <c r="AV209" s="1"/>
+      <c r="AW209" s="1"/>
+      <c r="AX209" s="1"/>
+      <c r="AY209" s="1"/>
+      <c r="AZ209" s="1"/>
+      <c r="BA209" s="1"/>
+      <c r="BB209" s="1"/>
+      <c r="BC209" s="1"/>
+      <c r="BD209" s="1"/>
+      <c r="BE209" s="1"/>
+      <c r="BF209" s="1"/>
+      <c r="BG209" s="1"/>
+      <c r="BH209" s="1"/>
+      <c r="BI209" s="11"/>
+      <c r="BJ209" s="1"/>
+      <c r="BK209" s="1"/>
+      <c r="BL209" s="1"/>
+      <c r="BM209" s="1"/>
+      <c r="BN209" s="1"/>
+      <c r="BO209" s="1"/>
+      <c r="BP209" s="1"/>
+      <c r="BQ209" s="1"/>
+      <c r="BR209" s="1"/>
+      <c r="BS209" s="1"/>
+      <c r="BT209" s="1"/>
+      <c r="BU209" s="1"/>
+      <c r="BV209" s="1"/>
+      <c r="BW209" s="1"/>
+      <c r="BX209" s="1"/>
+      <c r="BY209" s="1"/>
+      <c r="BZ209" s="1"/>
+      <c r="CA209" s="1"/>
+      <c r="CB209" s="1"/>
+      <c r="CC209" s="1"/>
+      <c r="CD209" s="1"/>
+      <c r="CE209" s="1"/>
+      <c r="CF209" s="1"/>
+      <c r="CG209" s="1"/>
     </row>
     <row r="210" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A210" s="8"/>
@@ -29763,7 +29870,7 @@
       <c r="CG271" s="2"/>
     </row>
     <row r="272" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A272" s="2"/>
+      <c r="A272" s="8"/>
       <c r="B272" s="2"/>
       <c r="C272" s="3"/>
       <c r="D272" s="2"/>
@@ -30632,6 +30739,93 @@
       <c r="CF281" s="2"/>
       <c r="CG281" s="2"/>
     </row>
+    <row r="282" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="A282" s="2"/>
+      <c r="B282" s="2"/>
+      <c r="C282" s="3"/>
+      <c r="D282" s="2"/>
+      <c r="E282" s="2"/>
+      <c r="F282" s="2"/>
+      <c r="G282" s="2"/>
+      <c r="H282" s="2"/>
+      <c r="I282" s="2"/>
+      <c r="J282" s="2"/>
+      <c r="K282" s="2"/>
+      <c r="L282" s="2"/>
+      <c r="M282" s="2"/>
+      <c r="N282" s="2"/>
+      <c r="O282" s="2"/>
+      <c r="P282" s="2"/>
+      <c r="Q282" s="2"/>
+      <c r="R282" s="2"/>
+      <c r="S282" s="2"/>
+      <c r="T282" s="2"/>
+      <c r="U282" s="2"/>
+      <c r="V282" s="2"/>
+      <c r="W282" s="2"/>
+      <c r="X282" s="2"/>
+      <c r="Y282" s="2"/>
+      <c r="Z282" s="2"/>
+      <c r="AA282" s="2"/>
+      <c r="AB282" s="2"/>
+      <c r="AC282" s="2"/>
+      <c r="AD282" s="2"/>
+      <c r="AE282" s="2"/>
+      <c r="AF282" s="2"/>
+      <c r="AG282" s="2"/>
+      <c r="AH282" s="2"/>
+      <c r="AI282" s="2"/>
+      <c r="AJ282" s="2"/>
+      <c r="AK282" s="2"/>
+      <c r="AL282" s="2"/>
+      <c r="AM282" s="2"/>
+      <c r="AN282" s="2"/>
+      <c r="AO282" s="2"/>
+      <c r="AP282" s="2"/>
+      <c r="AQ282" s="2"/>
+      <c r="AR282" s="2"/>
+      <c r="AS282" s="2"/>
+      <c r="AT282" s="2"/>
+      <c r="AU282" s="2"/>
+      <c r="AV282" s="2"/>
+      <c r="AW282" s="2"/>
+      <c r="AX282" s="2"/>
+      <c r="AY282" s="2"/>
+      <c r="AZ282" s="2"/>
+      <c r="BA282" s="2"/>
+      <c r="BB282" s="2"/>
+      <c r="BC282" s="2"/>
+      <c r="BD282" s="2"/>
+      <c r="BE282" s="2"/>
+      <c r="BF282" s="2"/>
+      <c r="BG282" s="2"/>
+      <c r="BH282" s="2"/>
+      <c r="BI282" s="3"/>
+      <c r="BJ282" s="2"/>
+      <c r="BK282" s="2"/>
+      <c r="BL282" s="2"/>
+      <c r="BM282" s="2"/>
+      <c r="BN282" s="2"/>
+      <c r="BO282" s="2"/>
+      <c r="BP282" s="2"/>
+      <c r="BQ282" s="2"/>
+      <c r="BR282" s="2"/>
+      <c r="BS282" s="2"/>
+      <c r="BT282" s="2"/>
+      <c r="BU282" s="2"/>
+      <c r="BV282" s="2"/>
+      <c r="BW282" s="2"/>
+      <c r="BX282" s="2"/>
+      <c r="BY282" s="2"/>
+      <c r="BZ282" s="2"/>
+      <c r="CA282" s="2"/>
+      <c r="CB282" s="2"/>
+      <c r="CC282" s="2"/>
+      <c r="CD282" s="2"/>
+      <c r="CE282" s="2"/>
+      <c r="CF282" s="2"/>
+      <c r="CG282" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink display="abc@test.com" r:id="rId1" ref="BM25"/>
@@ -30640,28 +30834,28 @@
     <hyperlink r:id="rId4" ref="C25"/>
     <hyperlink r:id="rId5" ref="C78"/>
     <hyperlink display="Ankit@12345" r:id="rId6" ref="AU78"/>
-    <hyperlink r:id="rId7" ref="C145"/>
-    <hyperlink display="Deepika@1234" r:id="rId8" ref="D145"/>
-    <hyperlink r:id="rId9" ref="C155"/>
-    <hyperlink r:id="rId10" ref="C156"/>
-    <hyperlink r:id="rId11" ref="C157"/>
-    <hyperlink r:id="rId12" ref="C158"/>
-    <hyperlink r:id="rId13" ref="C160"/>
-    <hyperlink r:id="rId14" ref="C151"/>
-    <hyperlink r:id="rId15" ref="C152"/>
-    <hyperlink r:id="rId16" ref="C153"/>
-    <hyperlink r:id="rId17" ref="C140"/>
-    <hyperlink r:id="rId18" ref="C141"/>
-    <hyperlink r:id="rId19" ref="AM130"/>
+    <hyperlink r:id="rId7" ref="C146"/>
+    <hyperlink display="Deepika@1234" r:id="rId8" ref="D146"/>
+    <hyperlink r:id="rId9" ref="C156"/>
+    <hyperlink r:id="rId10" ref="C157"/>
+    <hyperlink r:id="rId11" ref="C158"/>
+    <hyperlink r:id="rId12" ref="C159"/>
+    <hyperlink r:id="rId13" ref="C161"/>
+    <hyperlink r:id="rId14" ref="C152"/>
+    <hyperlink r:id="rId15" ref="C153"/>
+    <hyperlink r:id="rId16" ref="C154"/>
+    <hyperlink r:id="rId17" ref="C141"/>
+    <hyperlink r:id="rId18" ref="C142"/>
+    <hyperlink r:id="rId19" ref="AM131"/>
     <hyperlink r:id="rId20" ref="D11"/>
     <hyperlink r:id="rId21" ref="D83"/>
-    <hyperlink r:id="rId22" ref="C161"/>
-    <hyperlink r:id="rId23" ref="C162"/>
-    <hyperlink r:id="rId24" ref="C164"/>
-    <hyperlink r:id="rId25" ref="C165"/>
-    <hyperlink r:id="rId26" ref="C166"/>
-    <hyperlink r:id="rId27" ref="C163"/>
-    <hyperlink r:id="rId28" ref="C167"/>
+    <hyperlink r:id="rId22" ref="C162"/>
+    <hyperlink r:id="rId23" ref="C163"/>
+    <hyperlink r:id="rId24" ref="C165"/>
+    <hyperlink r:id="rId25" ref="C166"/>
+    <hyperlink r:id="rId26" ref="C167"/>
+    <hyperlink r:id="rId27" ref="C164"/>
+    <hyperlink r:id="rId28" ref="C168"/>
     <hyperlink display="Ankit@123" r:id="rId29" ref="D46:D47"/>
     <hyperlink display="Ankit@123" r:id="rId30" ref="D50:D52"/>
     <hyperlink r:id="rId31" ref="D54"/>
@@ -30676,21 +30870,20 @@
     <hyperlink display="Ankit@123" r:id="rId40" ref="D84:D97"/>
     <hyperlink r:id="rId41" ref="D106"/>
     <hyperlink display="Ankit@123" r:id="rId42" ref="D110:D112"/>
-    <hyperlink display="Ankit@123" r:id="rId43" ref="D114:D121"/>
-    <hyperlink display="Ankit@123" r:id="rId44" ref="D123:D144"/>
-    <hyperlink display="Ankit@123" r:id="rId45" ref="D146:D149"/>
-    <hyperlink display="Ankit@123" r:id="rId46" ref="D154:D158"/>
-    <hyperlink r:id="rId47" ref="D163"/>
-    <hyperlink display="Ankit@123" r:id="rId48" ref="D167:D170"/>
-    <hyperlink display="Ankit@123" r:id="rId49" ref="F155:F158"/>
-    <hyperlink r:id="rId50" ref="F163"/>
-    <hyperlink r:id="rId51" ref="F167"/>
+    <hyperlink display="Ankit@123" r:id="rId43" ref="D114:D122"/>
+    <hyperlink display="Ankit@123" r:id="rId44" ref="D124:D145"/>
+    <hyperlink display="Ankit@123" r:id="rId45" ref="D147:D150"/>
+    <hyperlink display="Ankit@123" r:id="rId46" ref="D155:D159"/>
+    <hyperlink r:id="rId47" ref="D164"/>
+    <hyperlink display="Ankit@123" r:id="rId48" ref="D168:D171"/>
+    <hyperlink display="Ankit@123" r:id="rId49" ref="F156:F159"/>
+    <hyperlink r:id="rId50" ref="F164"/>
+    <hyperlink r:id="rId51" ref="F168"/>
     <hyperlink r:id="rId52" ref="F66"/>
-    <hyperlink r:id="rId53" ref="C110"/>
-    <hyperlink display="Ankit@12345" r:id="rId54" ref="D78"/>
+    <hyperlink display="Ankit@12345" r:id="rId53" ref="D78"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId55"/>
+  <pageSetup orientation="portrait" r:id="rId54"/>
 </worksheet>
 </file>
 

</xml_diff>